<commit_message>
Update Angular Core 06 - Server Interaction - DucDV7 - Checklist.xlsx
</commit_message>
<xml_diff>
--- a/Angular Core 06 - Server Interaction - DucDV7 - Checklist.xlsx
+++ b/Angular Core 06 - Server Interaction - DucDV7 - Checklist.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hoc Tap Lap Trinh\Fsoft\CheckList JS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EC.Angular01\EC_Angular_Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Trainee</t>
   </si>
@@ -124,12 +124,16 @@
   </si>
   <si>
     <t>https://angular.io/guide/http</t>
+  </si>
+  <si>
+    <t>Ajax là từ viết tắt của các từ Asynchronus JavaScript và XML, là một nhóm các công nghệ phát triển web được sử dụng để tạo các ứng dụng để tạo các ứng dụng web động hay các ứng dụng giàu tính internet, hiểu đơn giản thì đây là công nghệ hoạt động kết hợp giữa JavaScript, XML và môi trường hoạt động bất đồng bộ.
+Bất đồng bộ ở đây được hiểu là khi có sự tương tác với website chỉ có một phần của website đó thay đổi mà không load lại hết trang web.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -226,8 +230,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -235,20 +248,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -288,7 +295,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -591,502 +598,496 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-    </row>
-    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="13" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+    </row>
+    <row r="26" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E29" s="9" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E29" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E30" s="9" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E31" s="9" t="s">
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E31" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E32" s="9" t="s">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E33" s="9" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E34" s="9" t="s">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E35" s="9" t="s">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:N24"/>
-    <mergeCell ref="C26:L26"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E27:J27"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="H29:J29"/>
@@ -1098,6 +1099,12 @@
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="H33:J33"/>
+    <mergeCell ref="A1:N24"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E27:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1107,28 +1114,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="6" max="6" width="107" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1161,8 +1169,11 @@
       <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1177,7 +1188,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1192,7 +1203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1209,7 +1220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1224,7 +1235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1236,7 +1247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1248,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1263,7 +1274,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1276,7 +1287,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
     </row>
   </sheetData>

</xml_diff>